<commit_message>
add README for Acknowledgements and References
</commit_message>
<xml_diff>
--- a/microcode.xlsx
+++ b/microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianrui.qi/Documents/LC2222a-ISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7724C1-4576-474E-8176-8C90D4E24B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3232E43E-762E-9C4B-9701-4A04F76E2036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,30 +809,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -851,7 +827,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1134,8 +1134,8 @@
   <dimension ref="A1:AS993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ20" sqref="AJ20"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1186,14 +1186,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
@@ -6352,24 +6352,24 @@
       <c r="A48" s="4"/>
     </row>
     <row r="49" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="46" t="s">
+      <c r="M49" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="N49" s="47"/>
-      <c r="O49" s="47"/>
-      <c r="P49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="49"/>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
@@ -6395,14 +6395,14 @@
       <c r="B50" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C50" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
       <c r="I50" s="1" t="s">
         <v>20</v>
       </c>
@@ -6447,14 +6447,14 @@
       <c r="B51" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C51" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
       <c r="I51" s="2" t="s">
         <v>59</v>
       </c>
@@ -6501,14 +6501,14 @@
       <c r="B52" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="55" t="s">
+      <c r="C52" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
       <c r="I52" s="14" t="s">
         <v>60</v>
       </c>
@@ -6608,17 +6608,17 @@
       </c>
     </row>
     <row r="56" spans="2:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
       <c r="L56" s="4"/>
       <c r="M56" s="12" t="s">
         <v>97</v>
@@ -6638,14 +6638,14 @@
       <c r="B57" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="51"/>
       <c r="I57" s="26" t="s">
         <v>20</v>
       </c>
@@ -6671,14 +6671,14 @@
       <c r="B58" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C58" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
       <c r="I58" s="30" t="s">
         <v>120</v>
       </c>
@@ -6705,14 +6705,14 @@
       <c r="B59" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="55" t="s">
+      <c r="C59" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
       <c r="I59" s="32" t="s">
         <v>121</v>
       </c>
@@ -6849,18 +6849,18 @@
     </row>
     <row r="67" spans="12:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L67" s="4"/>
-      <c r="M67" s="49"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="50"/>
-      <c r="P67" s="51"/>
+      <c r="M67" s="41"/>
+      <c r="N67" s="42"/>
+      <c r="O67" s="42"/>
+      <c r="P67" s="43"/>
       <c r="Q67" s="39"/>
     </row>
     <row r="68" spans="12:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L68" s="39"/>
-      <c r="M68" s="52"/>
-      <c r="N68" s="53"/>
-      <c r="O68" s="53"/>
-      <c r="P68" s="54"/>
+      <c r="M68" s="44"/>
+      <c r="N68" s="45"/>
+      <c r="O68" s="45"/>
+      <c r="P68" s="46"/>
       <c r="Q68" s="39"/>
       <c r="AS68" s="2"/>
     </row>
@@ -7809,17 +7809,17 @@
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="B56:J56"/>
     <mergeCell ref="M67:P68"/>
     <mergeCell ref="M49:P49"/>
     <mergeCell ref="C52:H52"/>
     <mergeCell ref="C57:H57"/>
     <mergeCell ref="C58:H58"/>
     <mergeCell ref="C59:H59"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="B56:J56"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="C2:H6 C8:H9 C11:H12 C14:H16 C18:H20 C22:H23 C25:H25 C27:H33 C35:H47">

</xml_diff>